<commit_message>
Avance de Fórmulas and Auditórias
</commit_message>
<xml_diff>
--- a/Calculos II Refencias Mixtas v2.xlsx
+++ b/Calculos II Refencias Mixtas v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Curso de Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CDB3C5-34A5-4FAE-B09B-BFED02113B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106F2264-9D02-4529-9D3C-42C5FDAECD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18195" yWindow="0" windowWidth="20205" windowHeight="21600" activeTab="4" xr2:uid="{905A9A7F-4C88-43F7-9E0A-9AE92DF99F55}"/>
+    <workbookView xWindow="15465" yWindow="0" windowWidth="22935" windowHeight="21600" activeTab="5" xr2:uid="{905A9A7F-4C88-43F7-9E0A-9AE92DF99F55}"/>
   </bookViews>
   <sheets>
     <sheet name="Fórmulas Básicas" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Copy Date" sheetId="2" r:id="rId3"/>
     <sheet name="Cálculosv4_Referencia" sheetId="4" r:id="rId4"/>
     <sheet name="TrimestreONETWOv5" sheetId="5" r:id="rId5"/>
+    <sheet name="CálculoAuditoríaV6" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="g">Cálculosv4_Referencia!$G$52</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="71">
   <si>
     <t>PRESUPUESTO COMPRAS MARZO 2019</t>
   </si>
@@ -167,6 +168,84 @@
   </si>
   <si>
     <t>Copiar y pegar</t>
+  </si>
+  <si>
+    <t>ALBARÁN</t>
+  </si>
+  <si>
+    <t>NOMBRE DE LA EMPRESA: ABMB S.A</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>ACTIVIDAD: MATERIAL INFORMÁTICO Y ELECTRODOMÉSTICOS</t>
+  </si>
+  <si>
+    <t>Descuento</t>
+  </si>
+  <si>
+    <t>NOMBRE DEL CLIENTE: SERVIPLUS  S.L.</t>
+  </si>
+  <si>
+    <t>I.V.A</t>
+  </si>
+  <si>
+    <t>CONCEPTO</t>
+  </si>
+  <si>
+    <t>UNIDADES</t>
+  </si>
+  <si>
+    <t>PRE/UNIDAD</t>
+  </si>
+  <si>
+    <t>DTO</t>
+  </si>
+  <si>
+    <t>Ordenador Pentium</t>
+  </si>
+  <si>
+    <t>Impresora de Inyección</t>
+  </si>
+  <si>
+    <t>Monitor</t>
+  </si>
+  <si>
+    <t>Televisor</t>
+  </si>
+  <si>
+    <t>Vídeo</t>
+  </si>
+  <si>
+    <t>Diskettes</t>
+  </si>
+  <si>
+    <t>CD_ROM</t>
+  </si>
+  <si>
+    <t>Tarjeta Controladora</t>
+  </si>
+  <si>
+    <t>Tarjeta VGA</t>
+  </si>
+  <si>
+    <t>Teclado</t>
+  </si>
+  <si>
+    <t>Filtros de pantalla</t>
+  </si>
+  <si>
+    <t>Ratón</t>
+  </si>
+  <si>
+    <t>Cable de impresora</t>
+  </si>
+  <si>
+    <t>Diskettera</t>
+  </si>
+  <si>
+    <t>Tarjeta de sonido</t>
   </si>
 </sst>
 </file>
@@ -275,7 +354,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -319,12 +398,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -341,13 +449,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -356,13 +462,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -760,13 +874,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -980,13 +1094,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
       <c r="I1" t="s">
         <v>15</v>
       </c>
@@ -1580,15 +1694,15 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1775,25 +1889,25 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="10" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1983,7 +2097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40EA1115-3345-4BC7-A66C-5523ED5C6726}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -2092,7 +2206,7 @@
         <v>300</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" ref="D9:D12" si="1">B10+C10</f>
+        <f t="shared" ref="D10:D12" si="1">B10+C10</f>
         <v>2156</v>
       </c>
     </row>
@@ -2194,4 +2308,464 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABA62436-F978-4784-B57E-AEC0C11E1FD3}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="21">
+        <f>SUM(F7:F21)</f>
+        <v>37496.144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="23">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="23">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1021.72</v>
+      </c>
+      <c r="D7">
+        <f>C7*I$3</f>
+        <v>91.954800000000006</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:E21" si="0">C7*I$4</f>
+        <v>214.56119999999999</v>
+      </c>
+      <c r="F7">
+        <f>(C7-D7+E7)*B7</f>
+        <v>1144.3263999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>414.7</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8:D21" si="1">C8*I$3</f>
+        <v>37.323</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>87.086999999999989</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ref="F8:F21" si="2">(C8-D8+E8)*B8</f>
+        <v>928.928</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>180.3</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>16.227</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>37.863</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>1009.6800000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>570.96</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>51.386400000000002</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>119.9016</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>5115.8016000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>420.71</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>37.863899999999994</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>88.349099999999993</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>3769.5616</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12">
+        <v>860</v>
+      </c>
+      <c r="C12">
+        <v>0.54</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>4.8600000000000004E-2</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.1134</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>520.12800000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>280.07</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>25.206299999999999</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>58.814699999999995</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>2823.1055999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14">
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>33.659999999999997</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>3.0293999999999994</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>7.0685999999999991</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>867.08159999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>28.25</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>2.5425</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>5.9325000000000001</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>348.04</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16">
+        <v>34</v>
+      </c>
+      <c r="C16">
+        <v>32.450000000000003</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>2.9205000000000001</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>6.8145000000000007</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>1235.6960000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17">
+        <v>56</v>
+      </c>
+      <c r="C17">
+        <v>66.11</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>5.9498999999999995</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>13.883099999999999</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>4146.4192000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18">
+        <v>67</v>
+      </c>
+      <c r="C18">
+        <v>23.44</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>2.1095999999999999</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>4.9223999999999997</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>1758.9376</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>5.89</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>0.5300999999999999</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>1.2368999999999999</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>59.371200000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20">
+        <v>123</v>
+      </c>
+      <c r="C20">
+        <v>31.25</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>2.8125</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>6.5625</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>4305</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21">
+        <v>74</v>
+      </c>
+      <c r="C21">
+        <v>114.19</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>10.277099999999999</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>23.979899999999997</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>9464.0671999999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <cellWatches>
+    <cellWatch r="H153"/>
+  </cellWatches>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Terminamos Referencias Mixtas v2
</commit_message>
<xml_diff>
--- a/Calculos II Refencias Mixtas v2.xlsx
+++ b/Calculos II Refencias Mixtas v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Curso de Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106F2264-9D02-4529-9D3C-42C5FDAECD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A916CBD-7E7C-45CC-8F91-32AF36890500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15465" yWindow="0" windowWidth="22935" windowHeight="21600" activeTab="5" xr2:uid="{905A9A7F-4C88-43F7-9E0A-9AE92DF99F55}"/>
+    <workbookView xWindow="15585" yWindow="0" windowWidth="22815" windowHeight="21600" activeTab="5" xr2:uid="{905A9A7F-4C88-43F7-9E0A-9AE92DF99F55}"/>
   </bookViews>
   <sheets>
     <sheet name="Fórmulas Básicas" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
   <si>
     <t>PRESUPUESTO COMPRAS MARZO 2019</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>Tarjeta de sonido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                  </t>
   </si>
 </sst>
 </file>
@@ -432,7 +435,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -450,6 +453,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -471,12 +478,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -874,13 +878,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1094,13 +1098,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
       <c r="I1" t="s">
         <v>15</v>
       </c>
@@ -1401,7 +1405,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B1" s="2"/>
@@ -1440,7 +1444,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
+      <c r="A2" s="17"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1479,7 +1483,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1518,7 +1522,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1568,7 +1572,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="9" t="s">
         <v>15</v>
       </c>
@@ -1694,15 +1698,15 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2104,12 +2108,12 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G2" t="s">
@@ -2174,12 +2178,12 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2249,12 +2253,12 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
@@ -2312,90 +2316,66 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABA62436-F978-4784-B57E-AEC0C11E1FD3}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="21">
+      <c r="I2" s="13">
         <f>SUM(F7:F21)</f>
-        <v>37496.144</v>
+        <v>37830.931000000004</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="23">
-        <v>0.09</v>
+      <c r="I3" s="8">
+        <v>0.08</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="8">
         <v>0.21</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2410,7 +2390,7 @@
       <c r="D6" t="s">
         <v>55</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="22" t="s">
         <v>15</v>
       </c>
       <c r="F6" t="s">
@@ -2429,15 +2409,15 @@
       </c>
       <c r="D7">
         <f>C7*I$3</f>
-        <v>91.954800000000006</v>
+        <v>81.7376</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E21" si="0">C7*I$4</f>
+        <f>C7*I$4</f>
         <v>214.56119999999999</v>
       </c>
       <c r="F7">
         <f>(C7-D7+E7)*B7</f>
-        <v>1144.3263999999999</v>
+        <v>1154.5436</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2451,16 +2431,16 @@
         <v>414.7</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:D21" si="1">C8*I$3</f>
-        <v>37.323</v>
+        <f>C8*I$3</f>
+        <v>33.176000000000002</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E8:E21" si="0">C8*I$4</f>
         <v>87.086999999999989</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:F21" si="2">(C8-D8+E8)*B8</f>
-        <v>928.928</v>
+        <f t="shared" ref="F8:F21" si="1">(C8-D8+E8)*B8</f>
+        <v>937.22199999999998</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2474,16 +2454,20 @@
         <v>180.3</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
-        <v>16.227</v>
+        <f>C9*I$3</f>
+        <v>14.424000000000001</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
         <v>37.863</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
-        <v>1009.6800000000001</v>
+        <f t="shared" si="1"/>
+        <v>1018.6950000000001</v>
+      </c>
+      <c r="H9" t="e">
+        <f>C7/0</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2497,16 +2481,16 @@
         <v>570.96</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
-        <v>51.386400000000002</v>
+        <f>C10*I$3</f>
+        <v>45.676800000000007</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
         <v>119.9016</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
-        <v>5115.8016000000007</v>
+        <f t="shared" si="1"/>
+        <v>5161.4784000000009</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2520,16 +2504,16 @@
         <v>420.71</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
-        <v>37.863899999999994</v>
+        <f>C11*I$3</f>
+        <v>33.656799999999997</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
         <v>88.349099999999993</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
-        <v>3769.5616</v>
+        <f t="shared" si="1"/>
+        <v>3803.2183999999997</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2543,16 +2527,16 @@
         <v>0.54</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
-        <v>4.8600000000000004E-2</v>
+        <f>C12*I$3</f>
+        <v>4.3200000000000002E-2</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
         <v>0.1134</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
-        <v>520.12800000000004</v>
+        <f t="shared" si="1"/>
+        <v>524.77200000000005</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2566,16 +2550,16 @@
         <v>280.07</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
-        <v>25.206299999999999</v>
+        <f>C13*I$3</f>
+        <v>22.4056</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
         <v>58.814699999999995</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
-        <v>2823.1055999999999</v>
+        <f t="shared" si="1"/>
+        <v>2848.3119000000002</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2589,16 +2573,16 @@
         <v>33.659999999999997</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
-        <v>3.0293999999999994</v>
+        <f>C14*I$3</f>
+        <v>2.6927999999999996</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
         <v>7.0685999999999991</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
-        <v>867.08159999999998</v>
+        <f t="shared" si="1"/>
+        <v>874.82339999999988</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2612,16 +2596,16 @@
         <v>28.25</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
-        <v>2.5425</v>
+        <f>C15*I$3</f>
+        <v>2.2600000000000002</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
         <v>5.9325000000000001</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
-        <v>348.04</v>
+        <f t="shared" si="1"/>
+        <v>351.14749999999998</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2635,19 +2619,19 @@
         <v>32.450000000000003</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
-        <v>2.9205000000000001</v>
+        <f>C16*I$3</f>
+        <v>2.5960000000000001</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
         <v>6.8145000000000007</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
-        <v>1235.6960000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1246.729</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -2658,19 +2642,19 @@
         <v>66.11</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
-        <v>5.9498999999999995</v>
+        <f>C17*I$3</f>
+        <v>5.2888000000000002</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
         <v>13.883099999999999</v>
       </c>
       <c r="F17">
-        <f t="shared" si="2"/>
-        <v>4146.4192000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>4183.4407999999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -2681,19 +2665,19 @@
         <v>23.44</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
-        <v>2.1095999999999999</v>
+        <f>C18*I$3</f>
+        <v>1.8752000000000002</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
         <v>4.9223999999999997</v>
       </c>
       <c r="F18">
-        <f t="shared" si="2"/>
-        <v>1758.9376</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1774.6424000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -2704,19 +2688,19 @@
         <v>5.89</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
-        <v>0.5300999999999999</v>
+        <f>C19*I$3</f>
+        <v>0.47120000000000001</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
         <v>1.2368999999999999</v>
       </c>
       <c r="F19">
-        <f t="shared" si="2"/>
-        <v>59.371200000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>59.901299999999992</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -2727,19 +2711,19 @@
         <v>31.25</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
-        <v>2.8125</v>
+        <f>C20*I$3</f>
+        <v>2.5</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
         <v>6.5625</v>
       </c>
       <c r="F20">
-        <f t="shared" si="2"/>
-        <v>4305</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>4343.4375</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>70</v>
       </c>
@@ -2750,22 +2734,28 @@
         <v>114.19</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
-        <v>10.277099999999999</v>
+        <f>C21*I$3</f>
+        <v>9.1351999999999993</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
         <v>23.979899999999997</v>
       </c>
       <c r="F21">
-        <f t="shared" si="2"/>
-        <v>9464.0671999999995</v>
+        <f t="shared" si="1"/>
+        <v>9548.5677999999989</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <cellWatches>
     <cellWatch r="H153"/>
+    <cellWatch r="F21"/>
   </cellWatches>
 </worksheet>
 </file>
</xml_diff>